<commit_message>
Adjust to only have a single node without any network
</commit_message>
<xml_diff>
--- a/data/markov/Power_BusInfo.xlsx
+++ b/data/markov/Power_BusInfo.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8803F9A3-E40A-458B-ACAB-F09F8B682B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B61BE0-50E7-4F62-B1A4-7539C58AED74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power BusInfo" sheetId="111" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power BusInfo'!$M$9:$R$13</definedName>
-    <definedName name="businfo">'Power BusInfo'!$B$3:$K$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power BusInfo'!$M$8:$R$11</definedName>
+    <definedName name="businfo">'Power BusInfo'!$B$3:$K$8</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
     <definedName name="dsmprofiles">#REF!</definedName>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -126,12 +126,6 @@
   </si>
   <si>
     <t>Node_1</t>
-  </si>
-  <si>
-    <t>Node_2</t>
-  </si>
-  <si>
-    <t>Node_3</t>
   </si>
   <si>
     <t>StylizedSystem</t>
@@ -727,9 +721,11 @@
   <sheetPr codeName="Tabelle9">
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:R13"/>
+  <dimension ref="B1:R11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -745,7 +741,7 @@
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
@@ -770,19 +766,19 @@
         <v>7</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -837,19 +833,19 @@
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -857,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="12">
         <v>220</v>
@@ -878,7 +874,7 @@
         <v>0.95</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K7" s="2">
         <v>2000</v>
@@ -894,82 +890,14 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="12">
-        <v>220</v>
-      </c>
-      <c r="E8" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0</v>
-      </c>
-      <c r="H8" s="12">
-        <v>0</v>
-      </c>
-      <c r="I8" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="2">
-        <v>2024</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="13">
-        <v>47.233400000000003</v>
-      </c>
-      <c r="N8" s="13">
-        <v>11.898199999999999</v>
-      </c>
+      <c r="M8" s="2"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
     </row>
-    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="12">
-        <v>220</v>
-      </c>
-      <c r="E9" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="G9" s="12">
-        <v>0</v>
-      </c>
-      <c r="H9" s="12">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" s="13">
-        <v>48.357199999999999</v>
-      </c>
-      <c r="N9" s="13">
-        <v>16.379300000000001</v>
-      </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="M9" s="2"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M10" s="2"/>
@@ -981,16 +909,6 @@
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M12" s="2"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M13" s="2"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -999,6 +917,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1144,15 +1071,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1160,6 +1078,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1173,14 +1099,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adjust markov quick example to new input
Add option to define output-file path for unit-commitment results
</commit_message>
<xml_diff>
--- a/data/markov/Power_BusInfo.xlsx
+++ b/data/markov/Power_BusInfo.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B61BE0-50E7-4F62-B1A4-7539C58AED74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE079F13-3B45-474D-A538-4366BB1A37D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Power BusInfo" sheetId="111" r:id="rId1"/>
+    <sheet name="ScenarioA" sheetId="111" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power BusInfo'!$M$8:$R$11</definedName>
-    <definedName name="businfo">'Power BusInfo'!$B$3:$K$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScenarioA!#REF!</definedName>
+    <definedName name="businfo">ScenarioA!$B$3:$O$8</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
     <definedName name="dsmprofiles">#REF!</definedName>
@@ -68,12 +68,55 @@
     <author>Felix Auer</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{7AF34EFF-DACA-4D71-A3B8-20A7BE1A49C5}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{854E4516-8C78-490E-A9CF-90F315F7ED05}">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If a line has a value in this column, it is not read in (i.e., does not exist).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{C0F21900-2458-4BD7-9609-B20AA15C2192}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Readable Name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{98F65EF8-751A-469D-9C6F-471F592122A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value specifier in DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{5B57641F-707D-47B6-A93B-5B7F518DBB94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -81,16 +124,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{90496568-61DD-449E-AA9F-EB2CD88BAC13}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{DB4D7B42-D0C4-40E1-9D51-E5E9F570E963}">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Source/ Typical Values</t>
+          <t>Details on database behavior</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{46C0FB7F-BD3D-4A7C-A461-EF92128E9E04}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit or valid values</t>
         </r>
       </text>
     </comment>
@@ -99,20 +157,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>[p.u.]</t>
   </si>
   <si>
-    <t>BaseVolt</t>
-  </si>
-  <si>
-    <t>maxVolt</t>
-  </si>
-  <si>
-    <t>minVolt</t>
-  </si>
-  <si>
     <t>Bs</t>
   </si>
   <si>
@@ -122,54 +171,200 @@
     <t>[kV]</t>
   </si>
   <si>
-    <t>PowerFactor</t>
-  </si>
-  <si>
     <t>Node_1</t>
   </si>
   <si>
+    <t>Power - Bus Info</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>[Year]</t>
+  </si>
+  <si>
+    <t>[°]</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Database ID</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>pBusBaseV</t>
+  </si>
+  <si>
+    <t>pBusMaxV</t>
+  </si>
+  <si>
+    <t>pBusMinV</t>
+  </si>
+  <si>
+    <t>Base Voltage</t>
+  </si>
+  <si>
+    <t>Max Voltage</t>
+  </si>
+  <si>
+    <t>Min Voltage</t>
+  </si>
+  <si>
+    <t>ID within database</t>
+  </si>
+  <si>
+    <t>Name of node</t>
+  </si>
+  <si>
+    <t>Zone in which node lies</t>
+  </si>
+  <si>
+    <t>Base voltage at node</t>
+  </si>
+  <si>
+    <t>Maximum voltage (in % of base voltage)</t>
+  </si>
+  <si>
+    <t>Minimum voltage (in % of base voltage)</t>
+  </si>
+  <si>
+    <t>pBusB</t>
+  </si>
+  <si>
+    <t>Conductance G connected to node</t>
+  </si>
+  <si>
+    <t>pBusG</t>
+  </si>
+  <si>
+    <t>Power Factor</t>
+  </si>
+  <si>
+    <t>pBus_pf</t>
+  </si>
+  <si>
+    <t>Power factor at node</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Commission Year</t>
+  </si>
+  <si>
+    <t>Decommission Year</t>
+  </si>
+  <si>
+    <t>[db-key]</t>
+  </si>
+  <si>
+    <t>[Node]</t>
+  </si>
+  <si>
+    <t>[Zone]</t>
+  </si>
+  <si>
+    <t>Is in zone of interest?</t>
+  </si>
+  <si>
+    <t>zoi</t>
+  </si>
+  <si>
+    <t>Data Package</t>
+  </si>
+  <si>
+    <t>dataPackage</t>
+  </si>
+  <si>
+    <t>[DataPackage]</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>dataSource</t>
+  </si>
+  <si>
+    <t>Where the data for the entry comes from</t>
+  </si>
+  <si>
+    <t>[DataSource]</t>
+  </si>
+  <si>
+    <t>Filled automatically by database</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Scenario-dependent</t>
+  </si>
+  <si>
+    <t>Format:</t>
+  </si>
+  <si>
+    <t>Excl.</t>
+  </si>
+  <si>
+    <t>Which package this belongs to</t>
+  </si>
+  <si>
+    <t>Year where it is commissioned (1.1.xxxx)</t>
+  </si>
+  <si>
+    <t>Year where it is decommissioned (31.12.xxxx)</t>
+  </si>
+  <si>
+    <t>[0, 1]</t>
+  </si>
+  <si>
+    <t>Whether node is relevant for end result (1) or not (0)</t>
+  </si>
+  <si>
     <t>StylizedSystem</t>
   </si>
   <si>
-    <t>Power - Bus Info</t>
+    <t>Susceptance B connected to node</t>
+  </si>
+  <si>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>excl</t>
   </si>
   <si>
     <t>YearCom</t>
   </si>
   <si>
     <t>YearDecom</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>[Year]</t>
-  </si>
-  <si>
-    <t>[°]</t>
-  </si>
-  <si>
-    <t>[yes, no]</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>ZoneOfInterest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -210,64 +405,75 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Aptos"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Aptos"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF002060"/>
-      <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="0"/>
       <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,6 +521,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -340,7 +558,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -351,52 +569,85 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="8">
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
     <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
@@ -721,193 +972,339 @@
   <sheetPr codeName="Tabelle9">
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:R11"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16" style="4" customWidth="1"/>
-    <col min="4" max="10" width="11.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="5.140625" style="2" customWidth="1"/>
+    <col min="2" max="16" width="20" style="2" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
+    <row r="4" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="10">
+        <v>220</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="K8" s="19">
+        <v>2000</v>
+      </c>
+      <c r="L8" s="19">
+        <v>2023</v>
+      </c>
+      <c r="M8" s="25">
+        <v>47.272599999999997</v>
+      </c>
+      <c r="N8" s="25">
+        <v>11.471399999999999</v>
+      </c>
+      <c r="O8" s="19">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="2:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="12">
-        <v>220</v>
-      </c>
-      <c r="E7" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12">
-        <v>0.95</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2000</v>
-      </c>
-      <c r="L7" s="2">
-        <v>2023</v>
-      </c>
-      <c r="M7" s="13">
-        <v>47.272599999999997</v>
-      </c>
-      <c r="N7" s="13">
-        <v>11.471399999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M8" s="2"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M9" s="2"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M10" s="2"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M11" s="2"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>